<commit_message>
Update to create target variable out of data preparation observing the sales cost into 4 types of customers which needs to be modeled for building models
</commit_message>
<xml_diff>
--- a/ELGI.xlsx
+++ b/ELGI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PTPL0125\workbook_upskill\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PTPL0125\workbook_upskill\SalesAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F32B2A2-21FB-4CD5-A20F-F25F43290DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8279F236-E4FF-48D5-B2FD-0FDE9E6A140F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D200537-867B-47D6-85A9-DB5FCEB7A2F7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="region_category" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">region_category!$A$1:$M$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">region_category!$A$1:$N$137</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="55">
   <si>
     <t>Reciprocating compressors</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>December</t>
+  </si>
+  <si>
+    <t>Customer_type</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2F3CA6-D464-433A-B754-9413AD92EC41}">
-  <dimension ref="A1:M137"/>
+  <dimension ref="A1:N137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,9 +585,10 @@
     <col min="8" max="8" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -624,8 +628,11 @@
       <c r="M1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -667,8 +674,11 @@
         <f>(K2*L2)</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -710,8 +720,11 @@
         <f t="shared" ref="M3:M13" si="1">(K3*L3)</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -753,8 +766,11 @@
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -796,8 +812,11 @@
         <f t="shared" si="1"/>
         <v>5000</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -839,8 +858,11 @@
         <f t="shared" si="1"/>
         <v>7500</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -882,8 +904,11 @@
         <f t="shared" si="1"/>
         <v>10500</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -925,8 +950,11 @@
         <f t="shared" si="1"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -968,8 +996,11 @@
         <f t="shared" si="1"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1011,8 +1042,11 @@
         <f t="shared" si="1"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1054,8 +1088,11 @@
         <f t="shared" si="1"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1097,8 +1134,11 @@
         <f t="shared" si="1"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1140,8 +1180,11 @@
         <f t="shared" si="1"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1183,8 +1226,11 @@
         <f>(K14*L14)</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1226,8 +1272,11 @@
         <f t="shared" ref="M15:M21" si="3">(K15*L15)</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1269,8 +1318,11 @@
         <f t="shared" si="3"/>
         <v>3000</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1312,8 +1364,11 @@
         <f t="shared" si="3"/>
         <v>5000</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1355,8 +1410,11 @@
         <f t="shared" si="3"/>
         <v>7500</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1398,8 +1456,11 @@
         <f t="shared" si="3"/>
         <v>10500</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1441,8 +1502,11 @@
         <f t="shared" si="3"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1484,8 +1548,11 @@
         <f t="shared" si="3"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1527,8 +1594,11 @@
         <f t="shared" ref="M22:M137" si="5">(K22*L22)</f>
         <v>3000</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1570,8 +1640,11 @@
         <f t="shared" ref="M23:M28" si="7">(K23*L23)</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1613,8 +1686,11 @@
         <f t="shared" si="7"/>
         <v>7500</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1656,8 +1732,11 @@
         <f t="shared" si="7"/>
         <v>10500</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1699,8 +1778,11 @@
         <f t="shared" si="7"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1742,8 +1824,11 @@
         <f t="shared" si="7"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1785,8 +1870,11 @@
         <f t="shared" si="7"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1828,8 +1916,11 @@
         <f t="shared" si="5"/>
         <v>5000</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1871,8 +1962,11 @@
         <f t="shared" ref="M30:M33" si="9">(K30*L30)</f>
         <v>7500</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1914,8 +2008,11 @@
         <f t="shared" si="9"/>
         <v>10500</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1957,8 +2054,11 @@
         <f t="shared" si="9"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>8</v>
       </c>
@@ -2000,8 +2100,11 @@
         <f t="shared" si="9"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5</v>
       </c>
@@ -2043,8 +2146,11 @@
         <f t="shared" si="5"/>
         <v>7500</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>6</v>
       </c>
@@ -2086,8 +2192,11 @@
         <f t="shared" ref="M35:M39" si="11">(K35*L35)</f>
         <v>10500</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>7</v>
       </c>
@@ -2129,8 +2238,11 @@
         <f t="shared" si="11"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>8</v>
       </c>
@@ -2172,8 +2284,11 @@
         <f t="shared" si="11"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>9</v>
       </c>
@@ -2215,8 +2330,11 @@
         <f t="shared" si="11"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>10</v>
       </c>
@@ -2258,8 +2376,11 @@
         <f t="shared" si="11"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>6</v>
       </c>
@@ -2301,8 +2422,11 @@
         <f t="shared" si="5"/>
         <v>10500</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>7</v>
       </c>
@@ -2344,8 +2468,11 @@
         <f t="shared" ref="M41:M44" si="13">(K41*L41)</f>
         <v>14000</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>8</v>
       </c>
@@ -2387,8 +2514,11 @@
         <f t="shared" si="13"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>9</v>
       </c>
@@ -2430,8 +2560,11 @@
         <f t="shared" si="13"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>10</v>
       </c>
@@ -2473,8 +2606,11 @@
         <f t="shared" si="13"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>7</v>
       </c>
@@ -2516,8 +2652,11 @@
         <f t="shared" si="5"/>
         <v>14000</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>8</v>
       </c>
@@ -2559,8 +2698,11 @@
         <f t="shared" ref="M46:M49" si="15">(K46*L46)</f>
         <v>18000</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>9</v>
       </c>
@@ -2602,8 +2744,11 @@
         <f t="shared" si="15"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>10</v>
       </c>
@@ -2645,8 +2790,11 @@
         <f t="shared" si="15"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>11</v>
       </c>
@@ -2688,8 +2836,11 @@
         <f t="shared" si="15"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>8</v>
       </c>
@@ -2731,8 +2882,11 @@
         <f t="shared" si="5"/>
         <v>18000</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>9</v>
       </c>
@@ -2774,8 +2928,11 @@
         <f t="shared" ref="M51:M53" si="17">(K51*L51)</f>
         <v>22500</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>10</v>
       </c>
@@ -2817,8 +2974,11 @@
         <f t="shared" si="17"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>11</v>
       </c>
@@ -2860,8 +3020,11 @@
         <f t="shared" si="17"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>9</v>
       </c>
@@ -2903,8 +3066,11 @@
         <f t="shared" si="5"/>
         <v>22500</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>10</v>
       </c>
@@ -2946,8 +3112,11 @@
         <f t="shared" ref="M55:M57" si="19">(K55*L55)</f>
         <v>27500</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>11</v>
       </c>
@@ -2989,8 +3158,11 @@
         <f t="shared" si="19"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>12</v>
       </c>
@@ -3032,8 +3204,11 @@
         <f t="shared" si="19"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>10</v>
       </c>
@@ -3075,8 +3250,11 @@
         <f t="shared" si="5"/>
         <v>27500</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11</v>
       </c>
@@ -3118,8 +3296,11 @@
         <f t="shared" ref="M59:M60" si="21">(K59*L59)</f>
         <v>2400</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>12</v>
       </c>
@@ -3161,8 +3342,11 @@
         <f t="shared" si="21"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>11</v>
       </c>
@@ -3204,8 +3388,11 @@
         <f t="shared" si="5"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>12</v>
       </c>
@@ -3247,8 +3434,11 @@
         <f t="shared" si="5"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
@@ -3290,8 +3480,11 @@
         <f t="shared" si="5"/>
         <v>6300</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
@@ -3333,8 +3526,11 @@
         <f t="shared" ref="M64:M70" si="23">(K64*L64)</f>
         <v>8000</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>3</v>
       </c>
@@ -3376,8 +3572,11 @@
         <f t="shared" si="23"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>4</v>
       </c>
@@ -3419,8 +3618,11 @@
         <f t="shared" si="23"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>5</v>
       </c>
@@ -3462,8 +3664,11 @@
         <f t="shared" si="23"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>6</v>
       </c>
@@ -3505,8 +3710,11 @@
         <f t="shared" si="23"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>7</v>
       </c>
@@ -3548,8 +3756,11 @@
         <f t="shared" si="23"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>8</v>
       </c>
@@ -3591,8 +3802,11 @@
         <f t="shared" si="23"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2</v>
       </c>
@@ -3634,8 +3848,11 @@
         <f t="shared" si="5"/>
         <v>8000</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>3</v>
       </c>
@@ -3677,8 +3894,11 @@
         <f t="shared" ref="M72:M80" si="25">(K72*L72)</f>
         <v>9900</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>4</v>
       </c>
@@ -3720,8 +3940,11 @@
         <f t="shared" si="25"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>5</v>
       </c>
@@ -3763,8 +3986,11 @@
         <f t="shared" si="25"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>6</v>
       </c>
@@ -3806,8 +4032,11 @@
         <f t="shared" si="25"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>7</v>
       </c>
@@ -3849,8 +4078,11 @@
         <f t="shared" si="25"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>8</v>
       </c>
@@ -3892,8 +4124,11 @@
         <f t="shared" si="25"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>9</v>
       </c>
@@ -3935,8 +4170,11 @@
         <f t="shared" si="25"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>10</v>
       </c>
@@ -3978,8 +4216,11 @@
         <f t="shared" si="25"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>11</v>
       </c>
@@ -4021,8 +4262,11 @@
         <f t="shared" si="25"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>3</v>
       </c>
@@ -4064,8 +4308,11 @@
         <f t="shared" si="5"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>4</v>
       </c>
@@ -4107,8 +4354,11 @@
         <f t="shared" ref="M82:M88" si="27">(K82*L82)</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>5</v>
       </c>
@@ -4150,8 +4400,11 @@
         <f t="shared" si="27"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>6</v>
       </c>
@@ -4193,8 +4446,11 @@
         <f t="shared" si="27"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>7</v>
       </c>
@@ -4236,8 +4492,11 @@
         <f t="shared" si="27"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>8</v>
       </c>
@@ -4279,8 +4538,11 @@
         <f t="shared" si="27"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>9</v>
       </c>
@@ -4322,8 +4584,11 @@
         <f t="shared" si="27"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>10</v>
       </c>
@@ -4365,8 +4630,11 @@
         <f t="shared" si="27"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>4</v>
       </c>
@@ -4408,8 +4676,11 @@
         <f t="shared" si="5"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>5</v>
       </c>
@@ -4451,8 +4722,11 @@
         <f t="shared" ref="M90:M95" si="29">(K90*L90)</f>
         <v>800</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>6</v>
       </c>
@@ -4494,8 +4768,11 @@
         <f t="shared" si="29"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>7</v>
       </c>
@@ -4537,8 +4814,11 @@
         <f t="shared" si="29"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>8</v>
       </c>
@@ -4580,8 +4860,11 @@
         <f t="shared" si="29"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>9</v>
       </c>
@@ -4623,8 +4906,11 @@
         <f t="shared" si="29"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>10</v>
       </c>
@@ -4666,8 +4952,11 @@
         <f t="shared" si="29"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>5</v>
       </c>
@@ -4709,8 +4998,11 @@
         <f t="shared" si="5"/>
         <v>800</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>6</v>
       </c>
@@ -4752,8 +5044,11 @@
         <f t="shared" ref="M97:M103" si="31">(K97*L97)</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N97">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>7</v>
       </c>
@@ -4795,8 +5090,11 @@
         <f t="shared" si="31"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>8</v>
       </c>
@@ -4838,8 +5136,11 @@
         <f t="shared" si="31"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>9</v>
       </c>
@@ -4881,8 +5182,11 @@
         <f t="shared" si="31"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N100">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>10</v>
       </c>
@@ -4924,8 +5228,11 @@
         <f t="shared" si="31"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>11</v>
       </c>
@@ -4967,8 +5274,11 @@
         <f t="shared" si="31"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N102">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>12</v>
       </c>
@@ -5010,8 +5320,11 @@
         <f t="shared" si="31"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>6</v>
       </c>
@@ -5053,8 +5366,11 @@
         <f t="shared" si="5"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>7</v>
       </c>
@@ -5096,8 +5412,11 @@
         <f t="shared" ref="M105:M110" si="33">(K105*L105)</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>8</v>
       </c>
@@ -5139,8 +5458,11 @@
         <f t="shared" si="33"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>9</v>
       </c>
@@ -5182,8 +5504,11 @@
         <f t="shared" si="33"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>10</v>
       </c>
@@ -5225,8 +5550,11 @@
         <f t="shared" si="33"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>11</v>
       </c>
@@ -5268,8 +5596,11 @@
         <f t="shared" si="33"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>12</v>
       </c>
@@ -5311,8 +5642,11 @@
         <f t="shared" si="33"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>7</v>
       </c>
@@ -5354,8 +5688,11 @@
         <f t="shared" si="5"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>8</v>
       </c>
@@ -5397,8 +5734,11 @@
         <f t="shared" ref="M112:M116" si="35">(K112*L112)</f>
         <v>2400</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>9</v>
       </c>
@@ -5440,8 +5780,11 @@
         <f t="shared" si="35"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N113">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>10</v>
       </c>
@@ -5483,8 +5826,11 @@
         <f t="shared" si="35"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>11</v>
       </c>
@@ -5526,8 +5872,11 @@
         <f t="shared" si="35"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>12</v>
       </c>
@@ -5569,8 +5918,11 @@
         <f t="shared" si="35"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>8</v>
       </c>
@@ -5612,8 +5964,11 @@
         <f t="shared" si="5"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>9</v>
       </c>
@@ -5655,8 +6010,11 @@
         <f t="shared" ref="M118:M121" si="37">(K118*L118)</f>
         <v>3500</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>10</v>
       </c>
@@ -5698,8 +6056,11 @@
         <f t="shared" si="37"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>11</v>
       </c>
@@ -5741,8 +6102,11 @@
         <f t="shared" si="37"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N120">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>12</v>
       </c>
@@ -5784,8 +6148,11 @@
         <f t="shared" si="37"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>9</v>
       </c>
@@ -5827,8 +6194,11 @@
         <f t="shared" si="5"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>10</v>
       </c>
@@ -5870,8 +6240,11 @@
         <f t="shared" ref="M123:M132" si="39">(K123*L123)</f>
         <v>9900</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>11</v>
       </c>
@@ -5913,8 +6286,11 @@
         <f t="shared" si="39"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N124">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>12</v>
       </c>
@@ -5956,8 +6332,11 @@
         <f t="shared" si="39"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>9</v>
       </c>
@@ -5999,8 +6378,11 @@
         <f t="shared" si="39"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>10</v>
       </c>
@@ -6042,8 +6424,11 @@
         <f t="shared" si="39"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>11</v>
       </c>
@@ -6085,8 +6470,11 @@
         <f t="shared" si="39"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>12</v>
       </c>
@@ -6128,8 +6516,11 @@
         <f t="shared" si="39"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>8</v>
       </c>
@@ -6171,8 +6562,11 @@
         <f t="shared" si="39"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>9</v>
       </c>
@@ -6214,8 +6608,11 @@
         <f t="shared" si="39"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>10</v>
       </c>
@@ -6257,8 +6654,11 @@
         <f t="shared" si="39"/>
         <v>9900</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>11</v>
       </c>
@@ -6300,8 +6700,11 @@
         <f t="shared" si="5"/>
         <v>12000</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>7</v>
       </c>
@@ -6343,8 +6746,11 @@
         <f t="shared" si="5"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>8</v>
       </c>
@@ -6386,8 +6792,11 @@
         <f t="shared" si="5"/>
         <v>2400</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>9</v>
       </c>
@@ -6429,8 +6838,11 @@
         <f t="shared" si="5"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>12</v>
       </c>
@@ -6471,6 +6883,9 @@
       <c r="M137">
         <f t="shared" si="5"/>
         <v>2400</v>
+      </c>
+      <c r="N137">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>